<commit_message>
DBG: Replace bias resistors of current measurement w/ correct part
And regenerate the CAM files.
</commit_message>
<xml_diff>
--- a/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs-debug_v1.1_formatted.xlsx
+++ b/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs-debug_v1.1_formatted.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35CA379A-6538-8A42-B907-B784D7FE3DE4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D73E9A-1560-7645-82BB-918C906FC5B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{9A3D47E2-0A81-EE4E-9058-1425A83F999A}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{32C8C098-F870-A142-A788-47E62B6324D2}" name="cs_debug_v1.1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs_debug_v1.1.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs_debug_v1.1.csv" tab="0" semicolon="1">
       <textFields count="98">
         <textField/>
         <textField/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="515" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="293">
   <si>
     <t>Qty</t>
   </si>
@@ -528,12 +528,6 @@
     <t>R16, R24, R25, R40</t>
   </si>
   <si>
-    <t>ERA-2AEB2491X</t>
-  </si>
-  <si>
-    <t>0,1%</t>
-  </si>
-  <si>
     <t>R20, R29, R36, R56</t>
   </si>
   <si>
@@ -1027,6 +1021,9 @@
   </si>
   <si>
     <t>﻿RS-187R05A2-DS MT RT</t>
+  </si>
+  <si>
+    <t>ERA-3AEB2493V</t>
   </si>
 </sst>
 </file>
@@ -1388,7 +1385,7 @@
   <dimension ref="A1:S71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K29" sqref="K29"/>
+      <selection activeCell="P32" sqref="P32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1487,10 +1484,10 @@
         <v>21</v>
       </c>
       <c r="K2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="L2" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
@@ -2367,10 +2364,10 @@
         <v>63</v>
       </c>
       <c r="L31" t="s">
-        <v>127</v>
-      </c>
-      <c r="P31" t="s">
-        <v>128</v>
+        <v>292</v>
+      </c>
+      <c r="P31" s="2">
+        <v>1E-3</v>
       </c>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.2">
@@ -2387,7 +2384,7 @@
         <v>61</v>
       </c>
       <c r="E32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -2396,7 +2393,7 @@
         <v>63</v>
       </c>
       <c r="L32" t="s">
-        <v>127</v>
+        <v>292</v>
       </c>
       <c r="P32" s="2">
         <v>1E-3</v>
@@ -2416,7 +2413,7 @@
         <v>61</v>
       </c>
       <c r="E33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F33" t="s">
         <v>45</v>
@@ -2425,7 +2422,7 @@
         <v>63</v>
       </c>
       <c r="L33" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="P33" s="1">
         <v>0.05</v>
@@ -2436,7 +2433,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C34" t="s">
         <v>60</v>
@@ -2445,7 +2442,7 @@
         <v>61</v>
       </c>
       <c r="E34" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="F34" t="s">
         <v>45</v>
@@ -2454,7 +2451,7 @@
         <v>63</v>
       </c>
       <c r="L34" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="P34" s="1">
         <v>0.05</v>
@@ -2465,28 +2462,28 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>133</v>
+      </c>
+      <c r="C35" t="s">
+        <v>133</v>
+      </c>
+      <c r="D35" t="s">
+        <v>134</v>
+      </c>
+      <c r="E35" t="s">
         <v>135</v>
       </c>
-      <c r="C35" t="s">
-        <v>135</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="F35" t="s">
         <v>136</v>
       </c>
-      <c r="E35" t="s">
+      <c r="I35" t="s">
         <v>137</v>
       </c>
-      <c r="F35" t="s">
+      <c r="L35" t="s">
+        <v>133</v>
+      </c>
+      <c r="N35" t="s">
         <v>138</v>
-      </c>
-      <c r="I35" t="s">
-        <v>139</v>
-      </c>
-      <c r="L35" t="s">
-        <v>135</v>
-      </c>
-      <c r="N35" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:17" x14ac:dyDescent="0.2">
@@ -2494,7 +2491,7 @@
         <v>1</v>
       </c>
       <c r="B36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
         <v>60</v>
@@ -2503,7 +2500,7 @@
         <v>61</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="F36" t="s">
         <v>45</v>
@@ -2512,7 +2509,7 @@
         <v>63</v>
       </c>
       <c r="L36" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="P36" s="1">
         <v>0.05</v>
@@ -2523,25 +2520,25 @@
         <v>1</v>
       </c>
       <c r="B37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C37" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D37">
         <v>805</v>
       </c>
       <c r="E37" t="s">
+        <v>144</v>
+      </c>
+      <c r="F37" t="s">
+        <v>145</v>
+      </c>
+      <c r="K37" t="s">
         <v>146</v>
       </c>
-      <c r="F37" t="s">
-        <v>147</v>
-      </c>
-      <c r="K37" t="s">
-        <v>148</v>
-      </c>
       <c r="L37" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.2">
@@ -2549,25 +2546,25 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
+        <v>147</v>
+      </c>
+      <c r="C38" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" t="s">
         <v>149</v>
       </c>
-      <c r="C38" t="s">
+      <c r="E38" t="s">
         <v>150</v>
-      </c>
-      <c r="D38" t="s">
-        <v>151</v>
-      </c>
-      <c r="E38" t="s">
-        <v>152</v>
       </c>
       <c r="F38" t="s">
         <v>101</v>
       </c>
       <c r="J38" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.2">
@@ -2584,7 +2581,7 @@
         <v>61</v>
       </c>
       <c r="E39" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F39" t="s">
         <v>45</v>
@@ -2593,7 +2590,7 @@
         <v>63</v>
       </c>
       <c r="L39" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="P39" s="1">
         <v>0.05</v>
@@ -2613,7 +2610,7 @@
         <v>61</v>
       </c>
       <c r="E40" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="F40" t="s">
         <v>45</v>
@@ -2622,7 +2619,7 @@
         <v>63</v>
       </c>
       <c r="L40" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="P40" s="1">
         <v>0.05</v>
@@ -2633,7 +2630,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
         <v>60</v>
@@ -2642,7 +2639,7 @@
         <v>61</v>
       </c>
       <c r="E41" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F41" t="s">
         <v>45</v>
@@ -2651,7 +2648,7 @@
         <v>63</v>
       </c>
       <c r="L41" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="P41" s="1">
         <v>0.05</v>
@@ -2662,7 +2659,7 @@
         <v>3</v>
       </c>
       <c r="B42" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C42" t="s">
         <v>88</v>
@@ -2671,7 +2668,7 @@
         <v>89</v>
       </c>
       <c r="E42" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F42" t="s">
         <v>51</v>
@@ -2680,7 +2677,7 @@
         <v>52</v>
       </c>
       <c r="L42" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="O42" t="s">
         <v>116</v>
@@ -2697,16 +2694,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
+        <v>163</v>
+      </c>
+      <c r="C43" t="s">
+        <v>164</v>
+      </c>
+      <c r="D43" t="s">
         <v>165</v>
       </c>
-      <c r="C43" t="s">
+      <c r="E43" t="s">
         <v>166</v>
-      </c>
-      <c r="D43" t="s">
-        <v>167</v>
-      </c>
-      <c r="E43" t="s">
-        <v>168</v>
       </c>
       <c r="F43" t="s">
         <v>51</v>
@@ -2715,7 +2712,7 @@
         <v>52</v>
       </c>
       <c r="L43" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="O43" t="s">
         <v>116</v>
@@ -2735,13 +2732,13 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C44" t="s">
+        <v>168</v>
+      </c>
+      <c r="D44" t="s">
+        <v>169</v>
+      </c>
+      <c r="E44" t="s">
         <v>170</v>
-      </c>
-      <c r="D44" t="s">
-        <v>171</v>
-      </c>
-      <c r="E44" t="s">
-        <v>172</v>
       </c>
       <c r="F44" t="s">
         <v>45</v>
@@ -2750,7 +2747,7 @@
         <v>63</v>
       </c>
       <c r="L44" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="P44" s="1">
         <v>0.01</v>
@@ -2761,16 +2758,16 @@
         <v>2</v>
       </c>
       <c r="B45" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D45" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E45" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F45" t="s">
         <v>45</v>
@@ -2779,7 +2776,7 @@
         <v>63</v>
       </c>
       <c r="L45" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="P45" s="1">
         <v>0.05</v>
@@ -2790,7 +2787,7 @@
         <v>1</v>
       </c>
       <c r="B46" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C46" t="s">
         <v>60</v>
@@ -2799,7 +2796,7 @@
         <v>61</v>
       </c>
       <c r="E46" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F46" t="s">
         <v>45</v>
@@ -2808,7 +2805,7 @@
         <v>63</v>
       </c>
       <c r="L46" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="P46" s="1">
         <v>0.05</v>
@@ -2819,7 +2816,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C47" t="s">
         <v>60</v>
@@ -2828,7 +2825,7 @@
         <v>61</v>
       </c>
       <c r="E47" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F47" t="s">
         <v>45</v>
@@ -2837,7 +2834,7 @@
         <v>63</v>
       </c>
       <c r="L47" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="P47" s="1">
         <v>0.05</v>
@@ -2857,7 +2854,7 @@
         <v>61</v>
       </c>
       <c r="E48" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F48" t="s">
         <v>45</v>
@@ -2866,7 +2863,7 @@
         <v>63</v>
       </c>
       <c r="L48" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P48" s="1">
         <v>0.05</v>
@@ -2877,19 +2874,19 @@
         <v>1</v>
       </c>
       <c r="B49" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" t="s">
+        <v>184</v>
+      </c>
+      <c r="D49" t="s">
         <v>185</v>
       </c>
-      <c r="C49" t="s">
+      <c r="E49" t="s">
         <v>186</v>
       </c>
-      <c r="D49" t="s">
-        <v>187</v>
-      </c>
-      <c r="E49" t="s">
-        <v>188</v>
-      </c>
       <c r="L49" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.2">
@@ -2897,25 +2894,25 @@
         <v>1</v>
       </c>
       <c r="B50" t="s">
+        <v>187</v>
+      </c>
+      <c r="C50" t="s">
+        <v>188</v>
+      </c>
+      <c r="D50" t="s">
         <v>189</v>
       </c>
-      <c r="C50" t="s">
+      <c r="E50" t="s">
         <v>190</v>
       </c>
-      <c r="D50" t="s">
+      <c r="F50" t="s">
         <v>191</v>
       </c>
-      <c r="E50" t="s">
+      <c r="J50" t="s">
         <v>192</v>
       </c>
-      <c r="F50" t="s">
-        <v>193</v>
-      </c>
-      <c r="J50" t="s">
-        <v>194</v>
-      </c>
       <c r="L50" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.2">
@@ -2923,25 +2920,25 @@
         <v>1</v>
       </c>
       <c r="B51" t="s">
+        <v>193</v>
+      </c>
+      <c r="C51" t="s">
+        <v>193</v>
+      </c>
+      <c r="D51" t="s">
+        <v>194</v>
+      </c>
+      <c r="E51" t="s">
         <v>195</v>
       </c>
-      <c r="C51" t="s">
-        <v>195</v>
-      </c>
-      <c r="D51" t="s">
+      <c r="F51" t="s">
         <v>196</v>
       </c>
-      <c r="E51" t="s">
+      <c r="J51" t="s">
         <v>197</v>
       </c>
-      <c r="F51" t="s">
-        <v>198</v>
-      </c>
-      <c r="J51" t="s">
-        <v>199</v>
-      </c>
       <c r="L51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.2">
@@ -2949,19 +2946,19 @@
         <v>1</v>
       </c>
       <c r="B52" t="s">
+        <v>198</v>
+      </c>
+      <c r="C52" t="s">
+        <v>198</v>
+      </c>
+      <c r="D52" t="s">
+        <v>199</v>
+      </c>
+      <c r="E52" t="s">
         <v>200</v>
       </c>
-      <c r="C52" t="s">
-        <v>200</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="L52" t="s">
         <v>201</v>
-      </c>
-      <c r="E52" t="s">
-        <v>202</v>
-      </c>
-      <c r="L52" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="53" spans="1:13" x14ac:dyDescent="0.2">
@@ -2969,28 +2966,28 @@
         <v>1</v>
       </c>
       <c r="B53" t="s">
+        <v>202</v>
+      </c>
+      <c r="C53" t="s">
+        <v>202</v>
+      </c>
+      <c r="D53" t="s">
+        <v>203</v>
+      </c>
+      <c r="E53" t="s">
         <v>204</v>
       </c>
-      <c r="C53" t="s">
-        <v>204</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="F53" t="s">
         <v>205</v>
       </c>
-      <c r="E53" t="s">
-        <v>206</v>
-      </c>
-      <c r="F53" t="s">
-        <v>207</v>
-      </c>
       <c r="J53" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="K53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="L53" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.2">
@@ -2998,25 +2995,25 @@
         <v>4</v>
       </c>
       <c r="B54" t="s">
+        <v>206</v>
+      </c>
+      <c r="C54" t="s">
+        <v>206</v>
+      </c>
+      <c r="D54" t="s">
+        <v>207</v>
+      </c>
+      <c r="E54" t="s">
         <v>208</v>
       </c>
-      <c r="C54" t="s">
-        <v>208</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="F54" t="s">
         <v>209</v>
       </c>
-      <c r="E54" t="s">
-        <v>210</v>
-      </c>
-      <c r="F54" t="s">
-        <v>211</v>
-      </c>
       <c r="I54" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="L54" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.2">
@@ -3024,22 +3021,22 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
+        <v>210</v>
+      </c>
+      <c r="C55" t="s">
+        <v>210</v>
+      </c>
+      <c r="D55" t="s">
+        <v>211</v>
+      </c>
+      <c r="E55" t="s">
         <v>212</v>
       </c>
-      <c r="C55" t="s">
-        <v>212</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="F55" t="s">
         <v>213</v>
       </c>
-      <c r="E55" t="s">
-        <v>214</v>
-      </c>
-      <c r="F55" t="s">
-        <v>215</v>
-      </c>
       <c r="L55" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.2">
@@ -3047,22 +3044,22 @@
         <v>4</v>
       </c>
       <c r="B56" t="s">
+        <v>214</v>
+      </c>
+      <c r="C56" t="s">
+        <v>214</v>
+      </c>
+      <c r="D56" t="s">
+        <v>215</v>
+      </c>
+      <c r="E56" t="s">
         <v>216</v>
       </c>
-      <c r="C56" t="s">
-        <v>216</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="F56" t="s">
         <v>217</v>
       </c>
-      <c r="E56" t="s">
+      <c r="L56" t="s">
         <v>218</v>
-      </c>
-      <c r="F56" t="s">
-        <v>219</v>
-      </c>
-      <c r="L56" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.2">
@@ -3070,25 +3067,25 @@
         <v>1</v>
       </c>
       <c r="B57" t="s">
+        <v>219</v>
+      </c>
+      <c r="C57" t="s">
+        <v>219</v>
+      </c>
+      <c r="D57" t="s">
+        <v>220</v>
+      </c>
+      <c r="E57" t="s">
         <v>221</v>
       </c>
-      <c r="C57" t="s">
-        <v>221</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="F57" t="s">
         <v>222</v>
       </c>
-      <c r="E57" t="s">
+      <c r="J57" t="s">
         <v>223</v>
       </c>
-      <c r="F57" t="s">
+      <c r="L57" t="s">
         <v>224</v>
-      </c>
-      <c r="J57" t="s">
-        <v>225</v>
-      </c>
-      <c r="L57" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="58" spans="1:13" x14ac:dyDescent="0.2">
@@ -3096,25 +3093,25 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
+        <v>225</v>
+      </c>
+      <c r="C58" t="s">
+        <v>225</v>
+      </c>
+      <c r="D58" t="s">
+        <v>226</v>
+      </c>
+      <c r="E58" t="s">
         <v>227</v>
       </c>
-      <c r="C58" t="s">
-        <v>227</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="F58" t="s">
         <v>228</v>
       </c>
-      <c r="E58" t="s">
+      <c r="J58" t="s">
         <v>229</v>
       </c>
-      <c r="F58" t="s">
+      <c r="L58" t="s">
         <v>230</v>
-      </c>
-      <c r="J58" t="s">
-        <v>231</v>
-      </c>
-      <c r="L58" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.2">
@@ -3122,22 +3119,22 @@
         <v>1</v>
       </c>
       <c r="B59" t="s">
+        <v>231</v>
+      </c>
+      <c r="C59" t="s">
+        <v>231</v>
+      </c>
+      <c r="D59" t="s">
+        <v>232</v>
+      </c>
+      <c r="E59" t="s">
         <v>233</v>
       </c>
-      <c r="C59" t="s">
-        <v>233</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="F59" t="s">
         <v>234</v>
       </c>
-      <c r="E59" t="s">
+      <c r="H59" t="s">
         <v>235</v>
-      </c>
-      <c r="F59" t="s">
-        <v>236</v>
-      </c>
-      <c r="H59" t="s">
-        <v>237</v>
       </c>
       <c r="L59" s="3">
         <v>632723300011</v>
@@ -3151,28 +3148,28 @@
         <v>1</v>
       </c>
       <c r="B60" t="s">
+        <v>236</v>
+      </c>
+      <c r="C60" t="s">
+        <v>236</v>
+      </c>
+      <c r="D60" t="s">
+        <v>237</v>
+      </c>
+      <c r="E60" t="s">
         <v>238</v>
       </c>
-      <c r="C60" t="s">
-        <v>238</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="F60" t="s">
         <v>239</v>
       </c>
-      <c r="E60" t="s">
+      <c r="J60" t="s">
         <v>240</v>
       </c>
-      <c r="F60" t="s">
+      <c r="L60" t="s">
         <v>241</v>
       </c>
-      <c r="J60" t="s">
+      <c r="M60" t="s">
         <v>242</v>
-      </c>
-      <c r="L60" t="s">
-        <v>243</v>
-      </c>
-      <c r="M60" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="61" spans="1:13" x14ac:dyDescent="0.2">
@@ -3180,22 +3177,22 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
+        <v>243</v>
+      </c>
+      <c r="C61" t="s">
+        <v>244</v>
+      </c>
+      <c r="D61" t="s">
         <v>245</v>
       </c>
-      <c r="C61" t="s">
+      <c r="E61" t="s">
         <v>246</v>
       </c>
-      <c r="D61" t="s">
+      <c r="F61" t="s">
         <v>247</v>
       </c>
-      <c r="E61" t="s">
+      <c r="L61" t="s">
         <v>248</v>
-      </c>
-      <c r="F61" t="s">
-        <v>249</v>
-      </c>
-      <c r="L61" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
@@ -3203,25 +3200,25 @@
         <v>1</v>
       </c>
       <c r="B62" t="s">
+        <v>249</v>
+      </c>
+      <c r="C62" t="s">
+        <v>249</v>
+      </c>
+      <c r="D62" t="s">
+        <v>250</v>
+      </c>
+      <c r="E62" t="s">
         <v>251</v>
       </c>
-      <c r="C62" t="s">
-        <v>251</v>
-      </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
         <v>252</v>
       </c>
-      <c r="E62" t="s">
-        <v>253</v>
-      </c>
-      <c r="F62" t="s">
-        <v>254</v>
-      </c>
       <c r="K62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="L62" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
@@ -3229,22 +3226,22 @@
         <v>1</v>
       </c>
       <c r="B63" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C63" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D63">
         <v>1812</v>
       </c>
       <c r="E63" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="F63" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L63" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
@@ -3252,25 +3249,25 @@
         <v>2</v>
       </c>
       <c r="B64" t="s">
+        <v>257</v>
+      </c>
+      <c r="C64" t="s">
+        <v>257</v>
+      </c>
+      <c r="D64" t="s">
+        <v>258</v>
+      </c>
+      <c r="E64" t="s">
         <v>259</v>
       </c>
-      <c r="C64" t="s">
-        <v>259</v>
-      </c>
-      <c r="D64" t="s">
+      <c r="F64" t="s">
         <v>260</v>
       </c>
-      <c r="E64" t="s">
+      <c r="J64" t="s">
         <v>261</v>
       </c>
-      <c r="F64" t="s">
-        <v>262</v>
-      </c>
-      <c r="J64" t="s">
-        <v>263</v>
-      </c>
       <c r="L64" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.2">
@@ -3278,25 +3275,25 @@
         <v>2</v>
       </c>
       <c r="B65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="C65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="D65" t="s">
+        <v>258</v>
+      </c>
+      <c r="E65" t="s">
+        <v>262</v>
+      </c>
+      <c r="F65" t="s">
         <v>260</v>
       </c>
-      <c r="E65" t="s">
-        <v>264</v>
-      </c>
-      <c r="F65" t="s">
-        <v>262</v>
-      </c>
       <c r="J65" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="L65" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="66" spans="1:19" x14ac:dyDescent="0.2">
@@ -3304,22 +3301,22 @@
         <v>2</v>
       </c>
       <c r="B66" t="s">
+        <v>263</v>
+      </c>
+      <c r="C66" t="s">
+        <v>264</v>
+      </c>
+      <c r="D66" t="s">
         <v>265</v>
       </c>
-      <c r="C66" t="s">
+      <c r="E66" t="s">
         <v>266</v>
       </c>
-      <c r="D66" t="s">
+      <c r="F66" t="s">
         <v>267</v>
       </c>
-      <c r="E66" t="s">
-        <v>268</v>
-      </c>
-      <c r="F66" t="s">
-        <v>269</v>
-      </c>
       <c r="L66" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="67" spans="1:19" x14ac:dyDescent="0.2">
@@ -3327,25 +3324,25 @@
         <v>4</v>
       </c>
       <c r="B67" t="s">
+        <v>268</v>
+      </c>
+      <c r="C67" t="s">
+        <v>268</v>
+      </c>
+      <c r="D67" t="s">
+        <v>268</v>
+      </c>
+      <c r="E67" t="s">
+        <v>269</v>
+      </c>
+      <c r="F67" t="s">
         <v>270</v>
-      </c>
-      <c r="C67" t="s">
-        <v>270</v>
-      </c>
-      <c r="D67" t="s">
-        <v>270</v>
-      </c>
-      <c r="E67" t="s">
-        <v>271</v>
-      </c>
-      <c r="F67" t="s">
-        <v>272</v>
       </c>
       <c r="H67">
         <v>0.02</v>
       </c>
       <c r="L67" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="R67">
         <v>5.5</v>
@@ -3359,25 +3356,25 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
+        <v>271</v>
+      </c>
+      <c r="C68" t="s">
+        <v>272</v>
+      </c>
+      <c r="D68" t="s">
         <v>273</v>
       </c>
-      <c r="C68" t="s">
+      <c r="E68" t="s">
         <v>274</v>
       </c>
-      <c r="D68" t="s">
+      <c r="F68" t="s">
         <v>275</v>
       </c>
-      <c r="E68" t="s">
+      <c r="J68" t="s">
         <v>276</v>
       </c>
-      <c r="F68" t="s">
+      <c r="L68" t="s">
         <v>277</v>
-      </c>
-      <c r="J68" t="s">
-        <v>278</v>
-      </c>
-      <c r="L68" t="s">
-        <v>279</v>
       </c>
     </row>
     <row r="69" spans="1:19" x14ac:dyDescent="0.2">
@@ -3385,25 +3382,25 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
+        <v>278</v>
+      </c>
+      <c r="C69" t="s">
+        <v>278</v>
+      </c>
+      <c r="D69" t="s">
+        <v>279</v>
+      </c>
+      <c r="E69" t="s">
         <v>280</v>
       </c>
-      <c r="C69" t="s">
-        <v>280</v>
-      </c>
-      <c r="D69" t="s">
+      <c r="F69" t="s">
         <v>281</v>
       </c>
-      <c r="E69" t="s">
-        <v>282</v>
-      </c>
-      <c r="F69" t="s">
-        <v>283</v>
-      </c>
       <c r="J69" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="L69" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="70" spans="1:19" x14ac:dyDescent="0.2">
@@ -3411,19 +3408,19 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
+        <v>282</v>
+      </c>
+      <c r="C70" t="s">
+        <v>282</v>
+      </c>
+      <c r="D70" t="s">
+        <v>283</v>
+      </c>
+      <c r="E70" t="s">
         <v>284</v>
       </c>
-      <c r="C70" t="s">
-        <v>284</v>
-      </c>
-      <c r="D70" t="s">
-        <v>285</v>
-      </c>
-      <c r="E70" t="s">
-        <v>286</v>
-      </c>
       <c r="L70" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="71" spans="1:19" x14ac:dyDescent="0.2">
@@ -3431,25 +3428,25 @@
         <v>2</v>
       </c>
       <c r="B71" t="s">
+        <v>285</v>
+      </c>
+      <c r="C71" t="s">
+        <v>285</v>
+      </c>
+      <c r="D71" t="s">
+        <v>169</v>
+      </c>
+      <c r="E71" t="s">
+        <v>286</v>
+      </c>
+      <c r="F71" t="s">
         <v>287</v>
       </c>
-      <c r="C71" t="s">
-        <v>287</v>
-      </c>
-      <c r="D71" t="s">
-        <v>171</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="J71" t="s">
+        <v>261</v>
+      </c>
+      <c r="L71" t="s">
         <v>288</v>
-      </c>
-      <c r="F71" t="s">
-        <v>289</v>
-      </c>
-      <c r="J71" t="s">
-        <v>263</v>
-      </c>
-      <c r="L71" t="s">
-        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DBG: Fix DFM issues for 7PCB
</commit_message>
<xml_diff>
--- a/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs-debug_v1.1_formatted.xlsx
+++ b/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs-debug_v1.1_formatted.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E367F307-C8D7-5D49-BCE6-06390B4EEBCD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D82BD246-8169-3042-A14E-8C49783FE03A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8920" yWindow="-26120" windowWidth="39140" windowHeight="16940" xr2:uid="{3A1B7E2E-5091-E345-8C8D-B7E29F9F0181}"/>
+    <workbookView xWindow="-8940" yWindow="-26080" windowWidth="39140" windowHeight="16940" xr2:uid="{3A1B7E2E-5091-E345-8C8D-B7E29F9F0181}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="cs_debug_v1.1" localSheetId="0">Sheet1!$A$1:$AQ$72</definedName>
+    <definedName name="cs_debug_v1.1" localSheetId="0">Sheet1!$A$1:$AP$72</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +38,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{D91308EA-9BFA-0E42-8EC2-CD6E1726535E}" name="cs_debug_v1.1" type="6" refreshedVersion="6" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs_debug_v1.1.csv" tab="0" semicolon="1">
+    <textPr sourceFile="/Users/work-reese/hardware/commonsense/cs-hardware/debug/CAM/CS-debug_v1.1/CAMOutputs/Assembly/cs_debug_v1.1.csv" tab="0" semicolon="1">
       <textFields count="98">
         <textField/>
         <textField/>
@@ -145,7 +145,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="570" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="568" uniqueCount="341">
   <si>
     <t>Qty</t>
   </si>
@@ -174,9 +174,6 @@
     <t>PART_NO</t>
   </si>
   <si>
-    <t>PART_NUMBER</t>
-  </si>
-  <si>
     <t>PIN_COUNT</t>
   </si>
   <si>
@@ -982,9 +979,6 @@
   </si>
   <si>
     <t>MIC94164YCS-TR</t>
-  </si>
-  <si>
-    <t>MIC94164</t>
   </si>
   <si>
     <t>YES</t>
@@ -1531,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5E62AC8-D904-B248-AE8B-C69736F9E83E}">
-  <dimension ref="A1:AP72"/>
+  <dimension ref="A1:AO72"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H35" sqref="H35"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1547,40 +1541,39 @@
     <col min="7" max="7" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="20.33203125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="24.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="23" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="80.6640625" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="4.33203125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="26.1640625" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="26" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="38.1640625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="27" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="26.1640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="26" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="20" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="38.1640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="27" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="9" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1704,143 +1697,140 @@
       <c r="AO1" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" t="s">
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s">
+      <c r="I2" t="s">
         <v>44</v>
       </c>
-      <c r="I2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="3" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>47</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>48</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>49</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>50</v>
       </c>
-      <c r="I3" t="s">
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="4" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" t="s">
+        <v>52</v>
+      </c>
+      <c r="I4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="E5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" t="s">
         <v>52</v>
       </c>
-      <c r="F4" t="s">
-        <v>49</v>
-      </c>
-      <c r="G4" t="s">
-        <v>53</v>
-      </c>
-      <c r="I4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
+      <c r="I5" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" t="s">
         <v>46</v>
       </c>
-      <c r="D5" t="s">
-        <v>47</v>
-      </c>
-      <c r="E5" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" t="s">
-        <v>49</v>
-      </c>
-      <c r="G5" t="s">
-        <v>53</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="E6" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="6" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" t="s">
-        <v>47</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" t="s">
         <v>57</v>
       </c>
-      <c r="F6" t="s">
-        <v>49</v>
-      </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>58</v>
       </c>
-      <c r="I6" t="s">
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="7" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>60</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>61</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>62</v>
       </c>
-      <c r="F7" t="s">
+      <c r="H7" t="s">
         <v>63</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>64</v>
       </c>
-      <c r="I7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1848,787 +1838,787 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" t="s">
         <v>66</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>67</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>68</v>
       </c>
-      <c r="F8" t="s">
+      <c r="I8" t="s">
         <v>69</v>
       </c>
-      <c r="I8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>4</v>
       </c>
       <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
         <v>71</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>74</v>
       </c>
-      <c r="F9" t="s">
+      <c r="H9" t="s">
         <v>75</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>76</v>
       </c>
-      <c r="I9" t="s">
+      <c r="AA9" t="s">
         <v>77</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AE9" t="s">
         <v>78</v>
       </c>
-      <c r="AF9" t="s">
+      <c r="AM9" t="s">
         <v>79</v>
       </c>
-      <c r="AN9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>35</v>
       </c>
       <c r="B10" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" t="s">
         <v>71</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>72</v>
       </c>
-      <c r="D10" t="s">
-        <v>73</v>
-      </c>
       <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>74</v>
+      </c>
+      <c r="H10" t="s">
+        <v>75</v>
+      </c>
+      <c r="I10" t="s">
         <v>81</v>
       </c>
-      <c r="F10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" t="s">
+      <c r="AA10" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE10" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11" t="s">
         <v>82</v>
       </c>
-      <c r="AB10" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF10" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN10" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="11" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>1</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>83</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>84</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>85</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" t="s">
         <v>86</v>
       </c>
-      <c r="F11" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>87</v>
       </c>
-      <c r="I11" t="s">
-        <v>88</v>
-      </c>
-      <c r="AF11" s="1">
+      <c r="AE11" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="12" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
       <c r="B12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C12" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
         <v>89</v>
       </c>
-      <c r="C12" t="s">
-        <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>85</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" t="s">
+        <v>86</v>
+      </c>
+      <c r="I12" t="s">
         <v>90</v>
       </c>
-      <c r="F12" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" t="s">
-        <v>87</v>
-      </c>
-      <c r="I12" t="s">
-        <v>91</v>
-      </c>
-      <c r="AF12" s="1">
+      <c r="AE12" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="13" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>6</v>
       </c>
       <c r="B13" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E13" t="s">
         <v>92</v>
       </c>
-      <c r="C13" t="s">
-        <v>84</v>
-      </c>
-      <c r="D13" t="s">
-        <v>85</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>68</v>
+      </c>
+      <c r="H13" t="s">
+        <v>86</v>
+      </c>
+      <c r="I13" t="s">
         <v>93</v>
       </c>
-      <c r="F13" t="s">
-        <v>69</v>
-      </c>
-      <c r="H13" t="s">
-        <v>87</v>
-      </c>
-      <c r="I13" t="s">
-        <v>94</v>
-      </c>
-      <c r="AF13" s="1">
+      <c r="AE13" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D14" t="s">
         <v>84</v>
       </c>
-      <c r="D14" t="s">
-        <v>85</v>
-      </c>
       <c r="E14" t="s">
+        <v>94</v>
+      </c>
+      <c r="F14" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I14" t="s">
         <v>95</v>
       </c>
-      <c r="F14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" t="s">
-        <v>87</v>
-      </c>
-      <c r="I14" t="s">
-        <v>96</v>
-      </c>
-      <c r="AF14" s="1">
+      <c r="AE14" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="15" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D15" t="s">
         <v>84</v>
       </c>
-      <c r="D15" t="s">
-        <v>85</v>
-      </c>
       <c r="E15" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" t="s">
+        <v>68</v>
+      </c>
+      <c r="H15" t="s">
+        <v>86</v>
+      </c>
+      <c r="I15" t="s">
         <v>97</v>
       </c>
-      <c r="F15" t="s">
-        <v>69</v>
-      </c>
-      <c r="H15" t="s">
-        <v>87</v>
-      </c>
-      <c r="I15" t="s">
-        <v>98</v>
-      </c>
-      <c r="AF15" s="1">
+      <c r="AE15" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:42" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D16" t="s">
+        <v>84</v>
+      </c>
+      <c r="E16" t="s">
         <v>99</v>
       </c>
-      <c r="C16" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" t="s">
-        <v>85</v>
-      </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" t="s">
+        <v>86</v>
+      </c>
+      <c r="I16" t="s">
         <v>100</v>
       </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I16" t="s">
-        <v>101</v>
-      </c>
-      <c r="AF16" s="2">
+      <c r="AE16" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>4</v>
       </c>
       <c r="B17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C17" t="s">
+        <v>83</v>
+      </c>
+      <c r="D17" t="s">
         <v>84</v>
       </c>
-      <c r="D17" t="s">
-        <v>85</v>
-      </c>
       <c r="E17" t="s">
+        <v>101</v>
+      </c>
+      <c r="F17" t="s">
+        <v>68</v>
+      </c>
+      <c r="H17" t="s">
+        <v>86</v>
+      </c>
+      <c r="I17" t="s">
+        <v>100</v>
+      </c>
+      <c r="Y17" t="s">
         <v>102</v>
       </c>
-      <c r="F17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H17" t="s">
-        <v>87</v>
-      </c>
-      <c r="I17" t="s">
-        <v>101</v>
-      </c>
-      <c r="Z17" t="s">
+      <c r="AE17" s="2">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s">
+        <v>83</v>
+      </c>
+      <c r="D18" t="s">
+        <v>84</v>
+      </c>
+      <c r="E18" t="s">
         <v>103</v>
       </c>
-      <c r="AF17" s="2">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>1</v>
-      </c>
-      <c r="B18" t="s">
-        <v>99</v>
-      </c>
-      <c r="C18" t="s">
-        <v>84</v>
-      </c>
-      <c r="D18" t="s">
-        <v>85</v>
-      </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
+        <v>68</v>
+      </c>
+      <c r="H18" t="s">
+        <v>86</v>
+      </c>
+      <c r="I18" t="s">
         <v>104</v>
       </c>
-      <c r="F18" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" t="s">
-        <v>87</v>
-      </c>
-      <c r="I18" t="s">
-        <v>105</v>
-      </c>
-      <c r="AF18" s="1">
+      <c r="AE18" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>4</v>
       </c>
       <c r="B19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C19" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" t="s">
         <v>84</v>
       </c>
-      <c r="D19" t="s">
-        <v>85</v>
-      </c>
       <c r="E19" t="s">
+        <v>105</v>
+      </c>
+      <c r="F19" t="s">
+        <v>68</v>
+      </c>
+      <c r="H19" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" t="s">
         <v>106</v>
       </c>
-      <c r="F19" t="s">
-        <v>69</v>
-      </c>
-      <c r="H19" t="s">
-        <v>87</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="AE19" s="1">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="20" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
         <v>107</v>
       </c>
-      <c r="AF19" s="1">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="20" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>1</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
+        <v>71</v>
+      </c>
+      <c r="D20" t="s">
+        <v>72</v>
+      </c>
+      <c r="E20" t="s">
         <v>108</v>
       </c>
-      <c r="C20" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
+        <v>74</v>
+      </c>
+      <c r="H20" t="s">
+        <v>75</v>
+      </c>
+      <c r="I20" t="s">
         <v>109</v>
       </c>
-      <c r="F20" t="s">
+      <c r="AA20" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE20" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM20" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="21" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C21" t="s">
+        <v>112</v>
+      </c>
+      <c r="D21" t="s">
+        <v>113</v>
+      </c>
+      <c r="E21" t="s">
+        <v>114</v>
+      </c>
+      <c r="F21" t="s">
+        <v>74</v>
+      </c>
+      <c r="H21" t="s">
         <v>75</v>
       </c>
-      <c r="H20" t="s">
-        <v>76</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="I21" t="s">
+        <v>115</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE21" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM21" t="s">
         <v>110</v>
       </c>
-      <c r="AB20" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF20" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>112</v>
-      </c>
-      <c r="C21" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" t="s">
-        <v>114</v>
-      </c>
-      <c r="E21" t="s">
-        <v>115</v>
-      </c>
-      <c r="F21" t="s">
-        <v>75</v>
-      </c>
-      <c r="H21" t="s">
-        <v>76</v>
-      </c>
-      <c r="I21" t="s">
-        <v>116</v>
-      </c>
-      <c r="AB21" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF21" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN21" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
       <c r="B22" t="s">
+        <v>116</v>
+      </c>
+      <c r="C22" t="s">
         <v>117</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>118</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>119</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
+        <v>74</v>
+      </c>
+      <c r="H22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
         <v>120</v>
       </c>
-      <c r="F22" t="s">
-        <v>75</v>
-      </c>
-      <c r="H22" t="s">
-        <v>76</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="AA22" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE22" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM22" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="23" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
         <v>121</v>
       </c>
-      <c r="AB22" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF22" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN22" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>122</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>123</v>
       </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>124</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>125</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>126</v>
       </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>127</v>
       </c>
-      <c r="I23" t="s">
+      <c r="AG23" t="s">
         <v>128</v>
       </c>
-      <c r="AH23" t="s">
+    </row>
+    <row r="24" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
+        <v>83</v>
+      </c>
+      <c r="D24" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" t="s">
         <v>130</v>
       </c>
-      <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" t="s">
-        <v>85</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
+        <v>68</v>
+      </c>
+      <c r="H24" t="s">
+        <v>86</v>
+      </c>
+      <c r="I24" t="s">
         <v>131</v>
       </c>
-      <c r="F24" t="s">
-        <v>69</v>
-      </c>
-      <c r="H24" t="s">
-        <v>87</v>
-      </c>
-      <c r="I24" t="s">
-        <v>132</v>
-      </c>
-      <c r="AF24" s="1">
+      <c r="AE24" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>4</v>
       </c>
       <c r="B25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C25" t="s">
+        <v>112</v>
+      </c>
+      <c r="D25" t="s">
+        <v>113</v>
+      </c>
+      <c r="E25" t="s">
         <v>133</v>
       </c>
-      <c r="C25" t="s">
-        <v>113</v>
-      </c>
-      <c r="D25" t="s">
-        <v>114</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>74</v>
+      </c>
+      <c r="H25" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" t="s">
         <v>134</v>
       </c>
-      <c r="F25" t="s">
-        <v>75</v>
-      </c>
-      <c r="H25" t="s">
-        <v>76</v>
-      </c>
-      <c r="I25" t="s">
-        <v>135</v>
-      </c>
-      <c r="AB25" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF25" s="1">
+      <c r="AA25" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE25" s="1">
         <v>0.1</v>
       </c>
-      <c r="AN25" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="26" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM25" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
       <c r="B26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C26" t="s">
+        <v>71</v>
+      </c>
+      <c r="D26" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" t="s">
         <v>136</v>
       </c>
-      <c r="C26" t="s">
+      <c r="F26" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" t="s">
+        <v>75</v>
+      </c>
+      <c r="I26" t="s">
+        <v>137</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE26" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM26" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="27" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D27" t="s">
         <v>72</v>
       </c>
-      <c r="D26" t="s">
-        <v>73</v>
-      </c>
-      <c r="E26" t="s">
-        <v>137</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E27" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" t="s">
+        <v>74</v>
+      </c>
+      <c r="H27" t="s">
         <v>75</v>
       </c>
-      <c r="H26" t="s">
-        <v>76</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="I27" t="s">
+        <v>140</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE27" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM27" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="28" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>138</v>
       </c>
-      <c r="AB26" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF26" s="1">
+      <c r="C28" t="s">
+        <v>71</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" t="s">
+        <v>142</v>
+      </c>
+      <c r="F28" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" t="s">
+        <v>75</v>
+      </c>
+      <c r="I28" t="s">
+        <v>143</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE28" s="1">
         <v>0.1</v>
       </c>
-      <c r="AN26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C27" t="s">
-        <v>72</v>
-      </c>
-      <c r="D27" t="s">
-        <v>73</v>
-      </c>
-      <c r="E27" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="AM28" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>144</v>
+      </c>
+      <c r="C29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D29" t="s">
+        <v>113</v>
+      </c>
+      <c r="E29" t="s">
+        <v>145</v>
+      </c>
+      <c r="F29" t="s">
+        <v>74</v>
+      </c>
+      <c r="H29" t="s">
         <v>75</v>
       </c>
-      <c r="H27" t="s">
-        <v>76</v>
-      </c>
-      <c r="I27" t="s">
-        <v>141</v>
-      </c>
-      <c r="AB27" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF27" s="1">
+      <c r="I29" t="s">
+        <v>146</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>77</v>
+      </c>
+      <c r="AE29" s="1">
         <v>0.1</v>
       </c>
-      <c r="AN27" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" t="s">
-        <v>72</v>
-      </c>
-      <c r="D28" t="s">
-        <v>73</v>
-      </c>
-      <c r="E28" t="s">
-        <v>143</v>
-      </c>
-      <c r="F28" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" t="s">
-        <v>76</v>
-      </c>
-      <c r="I28" t="s">
-        <v>144</v>
-      </c>
-      <c r="AB28" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF28" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN28" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" t="s">
-        <v>145</v>
-      </c>
-      <c r="C29" t="s">
-        <v>113</v>
-      </c>
-      <c r="D29" t="s">
-        <v>114</v>
-      </c>
-      <c r="E29" t="s">
-        <v>146</v>
-      </c>
-      <c r="F29" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" t="s">
-        <v>76</v>
-      </c>
-      <c r="I29" t="s">
-        <v>147</v>
-      </c>
-      <c r="AB29" t="s">
-        <v>78</v>
-      </c>
-      <c r="AF29" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN29" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM29" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>6</v>
       </c>
       <c r="B30" t="s">
+        <v>147</v>
+      </c>
+      <c r="C30" t="s">
+        <v>117</v>
+      </c>
+      <c r="D30" t="s">
+        <v>118</v>
+      </c>
+      <c r="E30" t="s">
         <v>148</v>
       </c>
-      <c r="C30" t="s">
-        <v>118</v>
-      </c>
-      <c r="D30" t="s">
-        <v>119</v>
-      </c>
-      <c r="E30" t="s">
+      <c r="F30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H30" t="s">
+        <v>75</v>
+      </c>
+      <c r="I30" t="s">
         <v>149</v>
       </c>
-      <c r="F30" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" t="s">
-        <v>76</v>
-      </c>
-      <c r="I30" t="s">
-        <v>150</v>
-      </c>
-      <c r="AB30" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF30" s="1">
+      <c r="AA30" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE30" s="1">
         <v>0.1</v>
       </c>
-      <c r="AN30" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" t="s">
+        <v>150</v>
+      </c>
+      <c r="C31" t="s">
         <v>151</v>
       </c>
-      <c r="C31" t="s">
+      <c r="D31" t="s">
         <v>152</v>
       </c>
-      <c r="D31" t="s">
+      <c r="E31" t="s">
         <v>153</v>
       </c>
-      <c r="E31" t="s">
+      <c r="F31" t="s">
+        <v>68</v>
+      </c>
+      <c r="H31" t="s">
+        <v>86</v>
+      </c>
+      <c r="I31" t="s">
         <v>154</v>
       </c>
-      <c r="F31" t="s">
-        <v>69</v>
-      </c>
-      <c r="H31" t="s">
-        <v>87</v>
-      </c>
-      <c r="I31" t="s">
+      <c r="AE31" t="s">
         <v>155</v>
       </c>
-      <c r="AF31" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="B32" t="s">
+        <v>150</v>
+      </c>
+      <c r="C32" t="s">
         <v>151</v>
       </c>
-      <c r="C32" t="s">
+      <c r="D32" t="s">
         <v>152</v>
       </c>
-      <c r="D32" t="s">
-        <v>153</v>
-      </c>
       <c r="E32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F32" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H32" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I32" t="s">
-        <v>155</v>
-      </c>
-      <c r="AF32" s="2">
+        <v>154</v>
+      </c>
+      <c r="AE32" s="2">
         <v>1E-3</v>
       </c>
     </row>
-    <row r="33" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2636,179 +2626,179 @@
         <v>270</v>
       </c>
       <c r="C33" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" t="s">
         <v>84</v>
       </c>
-      <c r="D33" t="s">
-        <v>85</v>
-      </c>
       <c r="E33" t="s">
+        <v>157</v>
+      </c>
+      <c r="F33" t="s">
+        <v>68</v>
+      </c>
+      <c r="H33" t="s">
+        <v>86</v>
+      </c>
+      <c r="I33" t="s">
         <v>158</v>
       </c>
-      <c r="F33" t="s">
-        <v>69</v>
-      </c>
-      <c r="H33" t="s">
-        <v>87</v>
-      </c>
-      <c r="I33" t="s">
+      <c r="AE33" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="34" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
         <v>159</v>
       </c>
-      <c r="AF33" s="1">
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>84</v>
+      </c>
+      <c r="E34" t="s">
+        <v>160</v>
+      </c>
+      <c r="F34" t="s">
+        <v>68</v>
+      </c>
+      <c r="H34" t="s">
+        <v>86</v>
+      </c>
+      <c r="I34" t="s">
+        <v>161</v>
+      </c>
+      <c r="AE34" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="34" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" t="s">
-        <v>160</v>
-      </c>
-      <c r="C34" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" t="s">
-        <v>85</v>
-      </c>
-      <c r="E34" t="s">
-        <v>161</v>
-      </c>
-      <c r="F34" t="s">
-        <v>69</v>
-      </c>
-      <c r="H34" t="s">
-        <v>87</v>
-      </c>
-      <c r="I34" t="s">
-        <v>162</v>
-      </c>
-      <c r="AF34" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="35" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>4</v>
       </c>
       <c r="B35" t="s">
+        <v>162</v>
+      </c>
+      <c r="C35" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35" t="s">
         <v>163</v>
       </c>
-      <c r="C35" t="s">
-        <v>163</v>
-      </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>164</v>
       </c>
-      <c r="E35" t="s">
+      <c r="F35" t="s">
         <v>165</v>
       </c>
-      <c r="F35" t="s">
+      <c r="I35" t="s">
+        <v>167</v>
+      </c>
+      <c r="K35" t="s">
+        <v>168</v>
+      </c>
+      <c r="M35" t="s">
+        <v>169</v>
+      </c>
+      <c r="S35" t="s">
         <v>166</v>
       </c>
-      <c r="I35" t="s">
-        <v>168</v>
-      </c>
-      <c r="L35" t="s">
-        <v>169</v>
-      </c>
-      <c r="N35" t="s">
+      <c r="AB35" t="s">
         <v>170</v>
-      </c>
-      <c r="T35" t="s">
-        <v>167</v>
       </c>
       <c r="AC35" t="s">
         <v>171</v>
       </c>
-      <c r="AD35" t="s">
+    </row>
+    <row r="36" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="36" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
+        <v>83</v>
+      </c>
+      <c r="D36" t="s">
+        <v>84</v>
+      </c>
+      <c r="E36" t="s">
         <v>173</v>
       </c>
-      <c r="C36" t="s">
-        <v>84</v>
-      </c>
-      <c r="D36" t="s">
-        <v>85</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="F36" t="s">
+        <v>68</v>
+      </c>
+      <c r="H36" t="s">
+        <v>86</v>
+      </c>
+      <c r="I36" t="s">
         <v>174</v>
       </c>
-      <c r="F36" t="s">
-        <v>69</v>
-      </c>
-      <c r="H36" t="s">
-        <v>87</v>
-      </c>
-      <c r="I36" t="s">
+      <c r="AE36" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="37" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" t="s">
         <v>175</v>
       </c>
-      <c r="AF36" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="37" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>176</v>
-      </c>
-      <c r="C37" t="s">
-        <v>177</v>
       </c>
       <c r="D37">
         <v>805</v>
       </c>
       <c r="E37" t="s">
+        <v>177</v>
+      </c>
+      <c r="F37" t="s">
         <v>178</v>
       </c>
-      <c r="F37" t="s">
+      <c r="I37" t="s">
         <v>179</v>
       </c>
-      <c r="I37" t="s">
+      <c r="O37" t="s">
         <v>180</v>
       </c>
-      <c r="P37" t="s">
+      <c r="AG37" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" t="s">
         <v>181</v>
       </c>
-      <c r="AH37" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="38" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>182</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>183</v>
       </c>
-      <c r="D38" t="s">
+      <c r="E38" t="s">
         <v>184</v>
       </c>
-      <c r="E38" t="s">
+      <c r="F38" t="s">
+        <v>125</v>
+      </c>
+      <c r="H38" t="s">
         <v>185</v>
       </c>
-      <c r="F38" t="s">
-        <v>126</v>
-      </c>
-      <c r="H38" t="s">
+      <c r="I38" t="s">
         <v>186</v>
       </c>
-      <c r="I38" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="39" spans="1:40" x14ac:dyDescent="0.2">
+    </row>
+    <row r="39" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -2816,28 +2806,28 @@
         <v>39</v>
       </c>
       <c r="C39" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" t="s">
         <v>84</v>
       </c>
-      <c r="D39" t="s">
-        <v>85</v>
-      </c>
       <c r="E39" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="F39" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I39" t="s">
-        <v>190</v>
-      </c>
-      <c r="AF39" s="1">
+        <v>189</v>
+      </c>
+      <c r="AE39" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="40" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -2845,127 +2835,127 @@
         <v>39</v>
       </c>
       <c r="C40" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" t="s">
         <v>84</v>
       </c>
-      <c r="D40" t="s">
-        <v>85</v>
-      </c>
       <c r="E40" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="F40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H40" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I40" t="s">
-        <v>189</v>
-      </c>
-      <c r="AF40" s="1">
+        <v>188</v>
+      </c>
+      <c r="AE40" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="41" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41" t="s">
+        <v>191</v>
+      </c>
+      <c r="C41" t="s">
+        <v>83</v>
+      </c>
+      <c r="D41" t="s">
+        <v>84</v>
+      </c>
+      <c r="E41" t="s">
         <v>192</v>
       </c>
-      <c r="C41" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" t="s">
-        <v>85</v>
-      </c>
-      <c r="E41" t="s">
+      <c r="F41" t="s">
+        <v>68</v>
+      </c>
+      <c r="H41" t="s">
+        <v>86</v>
+      </c>
+      <c r="I41" t="s">
         <v>193</v>
       </c>
-      <c r="F41" t="s">
-        <v>69</v>
-      </c>
-      <c r="H41" t="s">
-        <v>87</v>
-      </c>
-      <c r="I41" t="s">
-        <v>194</v>
-      </c>
-      <c r="AF41" s="1">
+      <c r="AE41" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="42" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>3</v>
       </c>
       <c r="B42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" t="s">
+        <v>112</v>
+      </c>
+      <c r="D42" t="s">
+        <v>113</v>
+      </c>
+      <c r="E42" t="s">
         <v>195</v>
       </c>
-      <c r="C42" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" t="s">
-        <v>114</v>
-      </c>
-      <c r="E42" t="s">
+      <c r="F42" t="s">
+        <v>74</v>
+      </c>
+      <c r="H42" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" t="s">
         <v>196</v>
       </c>
-      <c r="F42" t="s">
+      <c r="AA42" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE42" s="1">
+        <v>0.1</v>
+      </c>
+      <c r="AM42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" t="s">
+        <v>197</v>
+      </c>
+      <c r="C43" t="s">
+        <v>198</v>
+      </c>
+      <c r="D43" t="s">
+        <v>199</v>
+      </c>
+      <c r="E43" t="s">
+        <v>200</v>
+      </c>
+      <c r="F43" t="s">
+        <v>74</v>
+      </c>
+      <c r="H43" t="s">
         <v>75</v>
       </c>
-      <c r="H42" t="s">
-        <v>76</v>
-      </c>
-      <c r="I42" t="s">
-        <v>197</v>
-      </c>
-      <c r="AB42" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF42" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="AN42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" t="s">
-        <v>198</v>
-      </c>
-      <c r="C43" t="s">
-        <v>199</v>
-      </c>
-      <c r="D43" t="s">
-        <v>200</v>
-      </c>
-      <c r="E43" t="s">
+      <c r="I43" t="s">
         <v>201</v>
       </c>
-      <c r="F43" t="s">
-        <v>75</v>
-      </c>
-      <c r="H43" t="s">
-        <v>76</v>
-      </c>
-      <c r="I43" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB43" t="s">
-        <v>142</v>
-      </c>
-      <c r="AF43" s="1">
+      <c r="AA43" t="s">
+        <v>141</v>
+      </c>
+      <c r="AE43" s="1">
         <v>0.2</v>
       </c>
-      <c r="AN43" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="44" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AM43" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>1</v>
       </c>
@@ -2973,28 +2963,28 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C44" t="s">
+        <v>151</v>
+      </c>
+      <c r="D44" t="s">
         <v>152</v>
       </c>
-      <c r="D44" t="s">
-        <v>153</v>
-      </c>
       <c r="E44" t="s">
+        <v>202</v>
+      </c>
+      <c r="F44" t="s">
+        <v>68</v>
+      </c>
+      <c r="H44" t="s">
+        <v>86</v>
+      </c>
+      <c r="I44" t="s">
         <v>203</v>
       </c>
-      <c r="F44" t="s">
-        <v>69</v>
-      </c>
-      <c r="H44" t="s">
-        <v>87</v>
-      </c>
-      <c r="I44" t="s">
-        <v>204</v>
-      </c>
-      <c r="AF44" s="1">
+      <c r="AE44" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="45" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>7</v>
       </c>
@@ -3002,115 +2992,115 @@
         <v>5.0999999999999996</v>
       </c>
       <c r="C45" t="s">
+        <v>151</v>
+      </c>
+      <c r="D45" t="s">
         <v>152</v>
       </c>
-      <c r="D45" t="s">
-        <v>153</v>
-      </c>
       <c r="E45" t="s">
+        <v>204</v>
+      </c>
+      <c r="F45" t="s">
+        <v>68</v>
+      </c>
+      <c r="H45" t="s">
+        <v>86</v>
+      </c>
+      <c r="I45" t="s">
         <v>205</v>
       </c>
-      <c r="F45" t="s">
-        <v>69</v>
-      </c>
-      <c r="H45" t="s">
-        <v>87</v>
-      </c>
-      <c r="I45" t="s">
-        <v>206</v>
-      </c>
-      <c r="AF45" s="1">
+      <c r="AE45" s="1">
         <v>0.01</v>
       </c>
     </row>
-    <row r="46" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:39" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
       <c r="B46" t="s">
+        <v>206</v>
+      </c>
+      <c r="C46" t="s">
+        <v>151</v>
+      </c>
+      <c r="D46" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" t="s">
         <v>207</v>
       </c>
-      <c r="C46" t="s">
-        <v>152</v>
-      </c>
-      <c r="D46" t="s">
-        <v>153</v>
-      </c>
-      <c r="E46" t="s">
+      <c r="F46" t="s">
+        <v>68</v>
+      </c>
+      <c r="H46" t="s">
+        <v>86</v>
+      </c>
+      <c r="I46" t="s">
         <v>208</v>
       </c>
-      <c r="F46" t="s">
-        <v>69</v>
-      </c>
-      <c r="H46" t="s">
-        <v>87</v>
-      </c>
-      <c r="I46" t="s">
+      <c r="AE46" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="47" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47" t="s">
         <v>209</v>
       </c>
-      <c r="AF46" s="1">
+      <c r="C47" t="s">
+        <v>83</v>
+      </c>
+      <c r="D47" t="s">
+        <v>84</v>
+      </c>
+      <c r="E47" t="s">
+        <v>210</v>
+      </c>
+      <c r="F47" t="s">
+        <v>68</v>
+      </c>
+      <c r="H47" t="s">
+        <v>86</v>
+      </c>
+      <c r="I47" t="s">
+        <v>211</v>
+      </c>
+      <c r="AE47" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="47" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>1</v>
-      </c>
-      <c r="B47" t="s">
-        <v>210</v>
-      </c>
-      <c r="C47" t="s">
+    <row r="48" spans="1:39" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
+        <v>212</v>
+      </c>
+      <c r="C48" t="s">
+        <v>83</v>
+      </c>
+      <c r="D48" t="s">
         <v>84</v>
       </c>
-      <c r="D47" t="s">
-        <v>85</v>
-      </c>
-      <c r="E47" t="s">
-        <v>211</v>
-      </c>
-      <c r="F47" t="s">
-        <v>69</v>
-      </c>
-      <c r="H47" t="s">
-        <v>87</v>
-      </c>
-      <c r="I47" t="s">
-        <v>212</v>
-      </c>
-      <c r="AF47" s="1">
+      <c r="E48" t="s">
+        <v>213</v>
+      </c>
+      <c r="F48" t="s">
+        <v>68</v>
+      </c>
+      <c r="H48" t="s">
+        <v>86</v>
+      </c>
+      <c r="I48" t="s">
+        <v>214</v>
+      </c>
+      <c r="AE48" s="1">
         <v>0.05</v>
       </c>
     </row>
-    <row r="48" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>1</v>
-      </c>
-      <c r="B48" t="s">
-        <v>213</v>
-      </c>
-      <c r="C48" t="s">
-        <v>84</v>
-      </c>
-      <c r="D48" t="s">
-        <v>85</v>
-      </c>
-      <c r="E48" t="s">
-        <v>214</v>
-      </c>
-      <c r="F48" t="s">
-        <v>69</v>
-      </c>
-      <c r="H48" t="s">
-        <v>87</v>
-      </c>
-      <c r="I48" t="s">
-        <v>215</v>
-      </c>
-      <c r="AF48" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>1</v>
       </c>
@@ -3118,698 +3108,692 @@
         <v>750</v>
       </c>
       <c r="C49" t="s">
+        <v>83</v>
+      </c>
+      <c r="D49" t="s">
         <v>84</v>
       </c>
-      <c r="D49" t="s">
-        <v>85</v>
-      </c>
       <c r="E49" t="s">
+        <v>215</v>
+      </c>
+      <c r="F49" t="s">
+        <v>68</v>
+      </c>
+      <c r="H49" t="s">
+        <v>86</v>
+      </c>
+      <c r="I49" t="s">
         <v>216</v>
       </c>
-      <c r="F49" t="s">
-        <v>69</v>
-      </c>
-      <c r="H49" t="s">
-        <v>87</v>
-      </c>
-      <c r="I49" t="s">
+      <c r="AE49" s="1">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="50" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>1</v>
+      </c>
+      <c r="B50" t="s">
         <v>217</v>
       </c>
-      <c r="AF49" s="1">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>1</v>
-      </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>218</v>
       </c>
-      <c r="C50" t="s">
+      <c r="D50" t="s">
         <v>219</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>220</v>
       </c>
-      <c r="E50" t="s">
+      <c r="I50" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="51" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>1</v>
+      </c>
+      <c r="B51" t="s">
         <v>221</v>
       </c>
-      <c r="I50" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>1</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>222</v>
       </c>
-      <c r="C51" t="s">
+      <c r="D51" t="s">
         <v>223</v>
       </c>
-      <c r="D51" t="s">
+      <c r="E51" t="s">
         <v>224</v>
       </c>
-      <c r="E51" t="s">
+      <c r="F51" t="s">
         <v>225</v>
       </c>
-      <c r="F51" t="s">
+      <c r="H51" t="s">
         <v>226</v>
       </c>
-      <c r="H51" t="s">
+      <c r="I51" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="52" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>1</v>
+      </c>
+      <c r="B52" t="s">
         <v>227</v>
       </c>
-      <c r="I51" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>1</v>
-      </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
+        <v>227</v>
+      </c>
+      <c r="D52" t="s">
         <v>228</v>
       </c>
-      <c r="C52" t="s">
-        <v>228</v>
-      </c>
-      <c r="D52" t="s">
+      <c r="E52" t="s">
         <v>229</v>
       </c>
-      <c r="E52" t="s">
+      <c r="F52" t="s">
         <v>230</v>
       </c>
-      <c r="F52" t="s">
+      <c r="H52" t="s">
         <v>231</v>
       </c>
-      <c r="H52" t="s">
+      <c r="I52" t="s">
+        <v>227</v>
+      </c>
+      <c r="J52">
+        <v>10</v>
+      </c>
+      <c r="AJ52" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="53" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
         <v>232</v>
       </c>
-      <c r="I52" t="s">
-        <v>228</v>
-      </c>
-      <c r="K52">
-        <v>10</v>
-      </c>
-      <c r="AK52" t="s">
+      <c r="C53" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>1</v>
-      </c>
-      <c r="B53" t="s">
+      <c r="D53" t="s">
         <v>233</v>
       </c>
-      <c r="C53" t="s">
-        <v>233</v>
-      </c>
-      <c r="D53" t="s">
+      <c r="E53" t="s">
         <v>234</v>
       </c>
-      <c r="E53" t="s">
+      <c r="I53" t="s">
         <v>235</v>
       </c>
-      <c r="I53" t="s">
+      <c r="AJ53" t="s">
         <v>236</v>
       </c>
-      <c r="AK53" t="s">
+    </row>
+    <row r="54" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>1</v>
+      </c>
+      <c r="B54" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>1</v>
-      </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" t="s">
         <v>238</v>
       </c>
-      <c r="C54" t="s">
-        <v>238</v>
-      </c>
-      <c r="D54" t="s">
+      <c r="E54" t="s">
         <v>239</v>
       </c>
-      <c r="E54" t="s">
+      <c r="F54" t="s">
         <v>240</v>
       </c>
-      <c r="F54" t="s">
-        <v>241</v>
-      </c>
       <c r="H54" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="I54" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="55" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>4</v>
       </c>
       <c r="B55" t="s">
+        <v>241</v>
+      </c>
+      <c r="C55" t="s">
+        <v>241</v>
+      </c>
+      <c r="D55" t="s">
         <v>242</v>
       </c>
-      <c r="C55" t="s">
-        <v>242</v>
-      </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>243</v>
       </c>
-      <c r="E55" t="s">
+      <c r="F55" t="s">
         <v>244</v>
       </c>
-      <c r="F55" t="s">
-        <v>245</v>
-      </c>
       <c r="H55" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="I55" t="s">
-        <v>242</v>
-      </c>
-      <c r="N55" t="s">
+        <v>241</v>
+      </c>
+      <c r="M55" t="s">
+        <v>169</v>
+      </c>
+      <c r="S55" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB55" t="s">
         <v>170</v>
-      </c>
-      <c r="T55" t="s">
-        <v>167</v>
       </c>
       <c r="AC55" t="s">
         <v>171</v>
       </c>
-      <c r="AD55" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="56" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>1</v>
       </c>
       <c r="B56" t="s">
+        <v>245</v>
+      </c>
+      <c r="C56" t="s">
+        <v>245</v>
+      </c>
+      <c r="D56" t="s">
         <v>246</v>
       </c>
-      <c r="C56" t="s">
-        <v>246</v>
-      </c>
-      <c r="D56" t="s">
+      <c r="E56" t="s">
         <v>247</v>
       </c>
-      <c r="E56" t="s">
+      <c r="F56" t="s">
         <v>248</v>
       </c>
-      <c r="F56" t="s">
+      <c r="H56" t="s">
+        <v>340</v>
+      </c>
+      <c r="I56" t="s">
         <v>249</v>
       </c>
-      <c r="H56" t="s">
-        <v>342</v>
-      </c>
-      <c r="I56" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
+    </row>
+    <row r="57" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>4</v>
       </c>
       <c r="B57" t="s">
+        <v>250</v>
+      </c>
+      <c r="C57" t="s">
+        <v>250</v>
+      </c>
+      <c r="D57" t="s">
         <v>251</v>
       </c>
-      <c r="C57" t="s">
-        <v>251</v>
-      </c>
-      <c r="D57" t="s">
+      <c r="E57" t="s">
         <v>252</v>
       </c>
-      <c r="E57" t="s">
+      <c r="F57" t="s">
         <v>253</v>
       </c>
-      <c r="F57" t="s">
+      <c r="H57" t="s">
+        <v>231</v>
+      </c>
+      <c r="I57" t="s">
         <v>254</v>
       </c>
-      <c r="H57" t="s">
-        <v>232</v>
-      </c>
-      <c r="I57" t="s">
+      <c r="AJ57" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="58" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>1</v>
+      </c>
+      <c r="B58" t="s">
         <v>255</v>
       </c>
-      <c r="AK57" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>1</v>
-      </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
+        <v>255</v>
+      </c>
+      <c r="D58" t="s">
         <v>256</v>
       </c>
-      <c r="C58" t="s">
-        <v>256</v>
-      </c>
-      <c r="D58" t="s">
+      <c r="E58" t="s">
         <v>257</v>
       </c>
-      <c r="E58" t="s">
+      <c r="F58" t="s">
         <v>258</v>
       </c>
-      <c r="F58" t="s">
+      <c r="H58" t="s">
         <v>259</v>
       </c>
-      <c r="H58" t="s">
+      <c r="I58" t="s">
         <v>260</v>
       </c>
-      <c r="I58" t="s">
+    </row>
+    <row r="59" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>1</v>
+      </c>
+      <c r="B59" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>1</v>
-      </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>261</v>
+      </c>
+      <c r="D59" t="s">
         <v>262</v>
       </c>
-      <c r="C59" t="s">
-        <v>262</v>
-      </c>
-      <c r="D59" t="s">
+      <c r="E59" t="s">
         <v>263</v>
       </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>264</v>
       </c>
-      <c r="F59" t="s">
+      <c r="H59" t="s">
         <v>265</v>
       </c>
-      <c r="H59" t="s">
+      <c r="I59" t="s">
         <v>266</v>
       </c>
-      <c r="I59" t="s">
+    </row>
+    <row r="60" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>1</v>
+      </c>
+      <c r="B60" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>1</v>
-      </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
+        <v>267</v>
+      </c>
+      <c r="D60" t="s">
         <v>268</v>
       </c>
-      <c r="C60" t="s">
-        <v>268</v>
-      </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>269</v>
       </c>
-      <c r="E60" t="s">
+      <c r="F60" t="s">
         <v>270</v>
       </c>
-      <c r="F60" t="s">
-        <v>271</v>
-      </c>
       <c r="H60" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="I60">
         <v>632723300011</v>
       </c>
-      <c r="J60">
-        <v>632723300011</v>
-      </c>
-      <c r="P60" t="s">
+      <c r="O60" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="61" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>1</v>
+      </c>
+      <c r="B61" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>1</v>
-      </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
+        <v>272</v>
+      </c>
+      <c r="D61" t="s">
         <v>273</v>
       </c>
-      <c r="C61" t="s">
-        <v>273</v>
-      </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>274</v>
       </c>
-      <c r="E61" t="s">
+      <c r="F61" t="s">
         <v>275</v>
       </c>
-      <c r="F61" t="s">
+      <c r="H61" t="s">
         <v>276</v>
       </c>
-      <c r="H61" t="s">
+      <c r="I61" t="s">
         <v>277</v>
       </c>
-      <c r="I61" t="s">
+      <c r="P61" t="s">
         <v>278</v>
       </c>
-      <c r="J61" t="s">
-        <v>279</v>
-      </c>
-      <c r="Q61" t="s">
-        <v>280</v>
-      </c>
-      <c r="X61" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
+      <c r="W61" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="62" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>2</v>
       </c>
       <c r="B62" t="s">
+        <v>279</v>
+      </c>
+      <c r="C62" t="s">
+        <v>280</v>
+      </c>
+      <c r="D62" t="s">
         <v>281</v>
       </c>
-      <c r="C62" t="s">
+      <c r="E62" t="s">
         <v>282</v>
       </c>
-      <c r="D62" t="s">
+      <c r="F62" t="s">
         <v>283</v>
       </c>
-      <c r="E62" t="s">
+      <c r="I62" t="s">
         <v>284</v>
       </c>
-      <c r="F62" t="s">
+    </row>
+    <row r="63" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>1</v>
+      </c>
+      <c r="B63" t="s">
         <v>285</v>
       </c>
-      <c r="I62" t="s">
+      <c r="C63" t="s">
+        <v>285</v>
+      </c>
+      <c r="D63" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>1</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="E63" t="s">
         <v>287</v>
       </c>
-      <c r="C63" t="s">
-        <v>287</v>
-      </c>
-      <c r="D63" t="s">
+      <c r="F63" t="s">
         <v>288</v>
       </c>
-      <c r="E63" t="s">
-        <v>289</v>
-      </c>
-      <c r="F63" t="s">
+      <c r="H63" t="s">
+        <v>338</v>
+      </c>
+      <c r="I63" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="64" spans="1:36" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>1</v>
+      </c>
+      <c r="B64" t="s">
         <v>290</v>
       </c>
-      <c r="H63" t="s">
-        <v>340</v>
-      </c>
-      <c r="I63" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
-      <c r="A64">
-        <v>1</v>
-      </c>
-      <c r="B64" t="s">
-        <v>292</v>
-      </c>
       <c r="C64" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D64">
         <v>1812</v>
       </c>
       <c r="E64" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="F64" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="I64" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="65" spans="1:42" x14ac:dyDescent="0.2">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="65" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
       <c r="B65" t="s">
+        <v>294</v>
+      </c>
+      <c r="C65" t="s">
+        <v>294</v>
+      </c>
+      <c r="D65" t="s">
+        <v>295</v>
+      </c>
+      <c r="E65" t="s">
         <v>296</v>
       </c>
-      <c r="C65" t="s">
-        <v>296</v>
-      </c>
-      <c r="D65" t="s">
+      <c r="F65" t="s">
         <v>297</v>
       </c>
-      <c r="E65" t="s">
+      <c r="H65" t="s">
         <v>298</v>
       </c>
-      <c r="F65" t="s">
-        <v>299</v>
-      </c>
-      <c r="H65" t="s">
-        <v>300</v>
-      </c>
       <c r="I65" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="66" spans="1:42" x14ac:dyDescent="0.2">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="66" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
       <c r="B66" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C66" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D66" t="s">
+        <v>295</v>
+      </c>
+      <c r="E66" t="s">
+        <v>299</v>
+      </c>
+      <c r="F66" t="s">
         <v>297</v>
       </c>
-      <c r="E66" t="s">
-        <v>301</v>
-      </c>
-      <c r="F66" t="s">
-        <v>299</v>
-      </c>
       <c r="H66" t="s">
+        <v>298</v>
+      </c>
+      <c r="I66" t="s">
+        <v>294</v>
+      </c>
+      <c r="Y66" t="s">
         <v>300</v>
       </c>
-      <c r="I66" t="s">
-        <v>296</v>
-      </c>
-      <c r="Z66" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="67" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="67" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
       <c r="B67" t="s">
+        <v>301</v>
+      </c>
+      <c r="C67" t="s">
+        <v>302</v>
+      </c>
+      <c r="D67" t="s">
         <v>303</v>
       </c>
-      <c r="C67" t="s">
+      <c r="E67" t="s">
         <v>304</v>
       </c>
-      <c r="D67" t="s">
+      <c r="F67" t="s">
         <v>305</v>
       </c>
-      <c r="E67" t="s">
+      <c r="I67" t="s">
         <v>306</v>
       </c>
-      <c r="F67" t="s">
+      <c r="O67" t="s">
         <v>307</v>
       </c>
-      <c r="I67" t="s">
+      <c r="U67" t="s">
         <v>308</v>
       </c>
-      <c r="P67" t="s">
-        <v>309</v>
-      </c>
-      <c r="V67" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="68" spans="1:42" x14ac:dyDescent="0.2">
+    </row>
+    <row r="68" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>4</v>
       </c>
       <c r="B68" t="s">
+        <v>309</v>
+      </c>
+      <c r="C68" t="s">
+        <v>309</v>
+      </c>
+      <c r="D68" t="s">
+        <v>309</v>
+      </c>
+      <c r="E68" t="s">
+        <v>310</v>
+      </c>
+      <c r="F68" t="s">
         <v>311</v>
       </c>
-      <c r="C68" t="s">
-        <v>311</v>
-      </c>
-      <c r="D68" t="s">
-        <v>311</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="H68" t="s">
+        <v>231</v>
+      </c>
+      <c r="I68" t="s">
+        <v>309</v>
+      </c>
+      <c r="M68" t="s">
         <v>312</v>
       </c>
-      <c r="F68" t="s">
+      <c r="Q68" t="s">
         <v>313</v>
       </c>
-      <c r="H68" t="s">
-        <v>232</v>
-      </c>
-      <c r="I68" t="s">
-        <v>311</v>
-      </c>
-      <c r="N68" t="s">
+      <c r="R68">
+        <v>1370004439</v>
+      </c>
+      <c r="S68" t="s">
         <v>314</v>
       </c>
-      <c r="R68" t="s">
+      <c r="T68">
+        <v>30</v>
+      </c>
+      <c r="V68">
+        <v>150</v>
+      </c>
+      <c r="Z68" t="s">
         <v>315</v>
       </c>
-      <c r="S68">
-        <v>1370004439</v>
-      </c>
-      <c r="T68" t="s">
+      <c r="AD68">
+        <v>-74</v>
+      </c>
+      <c r="AH68" t="s">
         <v>316</v>
       </c>
-      <c r="U68">
-        <v>30</v>
-      </c>
-      <c r="W68">
-        <v>150</v>
-      </c>
-      <c r="AA68" t="s">
+      <c r="AI68" t="s">
         <v>317</v>
       </c>
-      <c r="AE68">
-        <v>-74</v>
-      </c>
-      <c r="AI68" t="s">
+      <c r="AK68">
+        <v>8</v>
+      </c>
+      <c r="AL68">
+        <v>6.5</v>
+      </c>
+      <c r="AN68">
+        <v>5.5</v>
+      </c>
+      <c r="AO68">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="69" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A69">
+        <v>1</v>
+      </c>
+      <c r="B69" t="s">
         <v>318</v>
       </c>
-      <c r="AJ68" t="s">
+      <c r="C69" t="s">
         <v>319</v>
       </c>
-      <c r="AL68">
-        <v>8</v>
-      </c>
-      <c r="AM68">
-        <v>6.5</v>
-      </c>
-      <c r="AO68">
-        <v>5.5</v>
-      </c>
-      <c r="AP68">
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="69" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A69">
-        <v>1</v>
-      </c>
-      <c r="B69" t="s">
+      <c r="D69" t="s">
         <v>320</v>
       </c>
-      <c r="C69" t="s">
+      <c r="E69" t="s">
         <v>321</v>
       </c>
-      <c r="D69" t="s">
+      <c r="F69" t="s">
         <v>322</v>
       </c>
-      <c r="E69" t="s">
+      <c r="H69" t="s">
         <v>323</v>
       </c>
-      <c r="F69" t="s">
+      <c r="I69" t="s">
         <v>324</v>
       </c>
-      <c r="H69" t="s">
+    </row>
+    <row r="70" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A70">
+        <v>1</v>
+      </c>
+      <c r="B70" t="s">
         <v>325</v>
       </c>
-      <c r="I69" t="s">
+      <c r="C70" t="s">
+        <v>325</v>
+      </c>
+      <c r="D70" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="70" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A70">
-        <v>1</v>
-      </c>
-      <c r="B70" t="s">
+      <c r="E70" t="s">
         <v>327</v>
       </c>
-      <c r="C70" t="s">
-        <v>327</v>
-      </c>
-      <c r="D70" t="s">
+      <c r="F70" t="s">
         <v>328</v>
       </c>
-      <c r="E70" t="s">
+      <c r="H70" t="s">
+        <v>231</v>
+      </c>
+      <c r="I70" t="s">
+        <v>325</v>
+      </c>
+      <c r="AJ70" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="71" spans="1:41" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>1</v>
+      </c>
+      <c r="B71" t="s">
         <v>329</v>
       </c>
-      <c r="F70" t="s">
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71" t="s">
         <v>330</v>
       </c>
-      <c r="H70" t="s">
-        <v>232</v>
-      </c>
-      <c r="I70" t="s">
-        <v>327</v>
-      </c>
-      <c r="AK70" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="71" spans="1:42" x14ac:dyDescent="0.2">
-      <c r="A71">
-        <v>1</v>
-      </c>
-      <c r="B71" t="s">
+      <c r="E71" t="s">
         <v>331</v>
       </c>
-      <c r="C71" t="s">
-        <v>331</v>
-      </c>
-      <c r="D71" t="s">
+      <c r="H71" t="s">
+        <v>276</v>
+      </c>
+      <c r="I71" t="s">
+        <v>329</v>
+      </c>
+      <c r="X71" t="s">
         <v>332</v>
       </c>
-      <c r="E71" t="s">
-        <v>333</v>
-      </c>
-      <c r="H71" t="s">
-        <v>277</v>
-      </c>
-      <c r="I71" t="s">
-        <v>331</v>
-      </c>
-      <c r="Y71" t="s">
-        <v>334</v>
-      </c>
-      <c r="AK71" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="72" spans="1:42" x14ac:dyDescent="0.2">
+      <c r="AJ71" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="72" spans="1:41" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
       <c r="B72" t="s">
+        <v>333</v>
+      </c>
+      <c r="C72" t="s">
+        <v>333</v>
+      </c>
+      <c r="D72" t="s">
+        <v>152</v>
+      </c>
+      <c r="E72" t="s">
+        <v>334</v>
+      </c>
+      <c r="F72" t="s">
         <v>335</v>
       </c>
-      <c r="C72" t="s">
-        <v>335</v>
-      </c>
-      <c r="D72" t="s">
-        <v>153</v>
-      </c>
-      <c r="E72" t="s">
+      <c r="H72" t="s">
+        <v>298</v>
+      </c>
+      <c r="I72" t="s">
         <v>336</v>
-      </c>
-      <c r="F72" t="s">
-        <v>337</v>
-      </c>
-      <c r="H72" t="s">
-        <v>300</v>
-      </c>
-      <c r="I72" t="s">
-        <v>338</v>
       </c>
     </row>
   </sheetData>

</xml_diff>